<commit_message>
permirsimi i manualit per kataster
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/Regjistri-i-fletëparaqtjës-1.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/Regjistri-i-fletëparaqtjës-1.xlsx
@@ -715,8 +715,8 @@
   </sheetPr>
   <dimension ref="B1:P667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +814,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="9">
-        <v>275.38</v>
+        <v>122.22</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
te dhenat per kataster
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/Regjistri-i-fletëparaqtjës-1.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/Regjistri-i-fletëparaqtjës-1.xlsx
@@ -77,9 +77,6 @@
     <t>Banim Individual</t>
   </si>
   <si>
-    <t>O-72217092-00733-20-____-____</t>
-  </si>
-  <si>
     <t>Rr. Eqrem Çabej</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>HASHANË</t>
+  </si>
+  <si>
+    <t>O-72217092-03227-0-____-____</t>
   </si>
 </sst>
 </file>
@@ -715,8 +715,8 @@
   </sheetPr>
   <dimension ref="B1:P667"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,30 +808,30 @@
         <v>14</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="9">
         <v>122.22</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="20" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
       <c r="N4" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>8</v>

</xml_diff>